<commit_message>
Actualización jornada 7 e inicio jornada 8
</commit_message>
<xml_diff>
--- a/data/jornada_7_inicial.xlsx
+++ b/data/jornada_7_inicial.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>JOR. 6</t>
+          <t>JOR. 7</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -507,12 +507,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Armada</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>Puche</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Coquina</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -538,7 +538,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>JOR. 6</t>
+          <t>JOR. 7</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -546,12 +546,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Kike</t>
+          <t>Gonzo</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Armada</t>
+          <t>Coquina</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -577,7 +577,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>JOR. 6</t>
+          <t>JOR. 7</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -590,7 +590,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Gonzo</t>
+          <t>Kike</t>
         </is>
       </c>
       <c r="I4" t="n">

</xml_diff>